<commit_message>
finishing up recording the experiment data
</commit_message>
<xml_diff>
--- a/performance-test/Experiment Data.xlsx
+++ b/performance-test/Experiment Data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\logan\Documents\School-Related\MS\Spring 2019\DB\Project\wisconsin-benchmark\performance-test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{312589BD-85F6-443A-940C-73D58CF65694}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6CD9DAFC-69B8-4E67-AEF1-51AA9FA9C28B}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13276" xr2:uid="{139C03C4-4511-44A7-BDD9-FC1DDE7946CE}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="220" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="261" uniqueCount="76">
   <si>
     <t>experiment #</t>
   </si>
@@ -225,6 +225,39 @@
   </si>
   <si>
     <t>HUNDREDKTUP1 AGGREGATE ON evenOnePercent</t>
+  </si>
+  <si>
+    <t>4.a</t>
+  </si>
+  <si>
+    <t>Query 10 (see notes)</t>
+  </si>
+  <si>
+    <t>GEQO effort = 1</t>
+  </si>
+  <si>
+    <t>4.b</t>
+  </si>
+  <si>
+    <t>4.c</t>
+  </si>
+  <si>
+    <t>GEQO effort = 5</t>
+  </si>
+  <si>
+    <t>GEQO effort = 10</t>
+  </si>
+  <si>
+    <t>Query 10 (see notes) - 10m tuples</t>
+  </si>
+  <si>
+    <t>work_mem = 1 Mb</t>
+  </si>
+  <si>
+    <t>work_mem = 512 kB</t>
+  </si>
+  <si>
+    <t>work_mem = 4 Mb</t>
   </si>
 </sst>
 </file>
@@ -604,10 +637,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2AE55FD8-01CA-4A4F-9707-6997CCE57C9A}">
-  <dimension ref="A1:I145"/>
+  <dimension ref="A1:I177"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A126" workbookViewId="0">
-      <selection activeCell="D146" sqref="D146"/>
+    <sheetView tabSelected="1" topLeftCell="A149" workbookViewId="0">
+      <selection activeCell="D178" sqref="D178"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -2973,6 +3006,489 @@
         <v>162</v>
       </c>
     </row>
+    <row r="148" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A148" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="B148" t="s">
+        <v>72</v>
+      </c>
+      <c r="C148">
+        <v>1</v>
+      </c>
+      <c r="D148">
+        <v>12932</v>
+      </c>
+    </row>
+    <row r="149" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A149" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="B149" t="s">
+        <v>67</v>
+      </c>
+      <c r="C149">
+        <v>2</v>
+      </c>
+      <c r="D149">
+        <v>16544</v>
+      </c>
+    </row>
+    <row r="150" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A150" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="C150">
+        <v>3</v>
+      </c>
+      <c r="D150">
+        <v>15971</v>
+      </c>
+    </row>
+    <row r="151" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A151" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="C151">
+        <v>4</v>
+      </c>
+      <c r="D151">
+        <v>16082</v>
+      </c>
+    </row>
+    <row r="152" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A152" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="C152">
+        <v>5</v>
+      </c>
+      <c r="D152">
+        <v>14770</v>
+      </c>
+      <c r="E152" s="1">
+        <f>MAX(D148:D152)</f>
+        <v>16544</v>
+      </c>
+      <c r="F152" s="1">
+        <f>MIN(D148:D152)</f>
+        <v>12932</v>
+      </c>
+      <c r="G152" s="1">
+        <f>AVERAGE(D148:D152)</f>
+        <v>15259.8</v>
+      </c>
+      <c r="H152" s="1">
+        <f>_xlfn.STDEV.S(D148:D152)</f>
+        <v>1456.8411718509333</v>
+      </c>
+      <c r="I152" s="1">
+        <f>((SUM(D148:D152) - E152 - F152) / (COUNT(D148:D152) - 2))</f>
+        <v>15607.666666666666</v>
+      </c>
+    </row>
+    <row r="153" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A153" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="B153" t="s">
+        <v>66</v>
+      </c>
+      <c r="C153">
+        <v>1</v>
+      </c>
+      <c r="D153">
+        <v>12717</v>
+      </c>
+    </row>
+    <row r="154" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A154" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="B154" t="s">
+        <v>70</v>
+      </c>
+      <c r="C154">
+        <v>2</v>
+      </c>
+      <c r="D154">
+        <v>14357</v>
+      </c>
+    </row>
+    <row r="155" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A155" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="C155">
+        <v>3</v>
+      </c>
+      <c r="D155">
+        <v>14186</v>
+      </c>
+    </row>
+    <row r="156" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A156" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="C156">
+        <v>4</v>
+      </c>
+      <c r="D156">
+        <v>13227</v>
+      </c>
+    </row>
+    <row r="157" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A157" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="C157">
+        <v>5</v>
+      </c>
+      <c r="D157">
+        <v>12827</v>
+      </c>
+      <c r="E157" s="1">
+        <f>MAX(D153:D157)</f>
+        <v>14357</v>
+      </c>
+      <c r="F157" s="1">
+        <f>MIN(D153:D157)</f>
+        <v>12717</v>
+      </c>
+      <c r="G157" s="1">
+        <f>AVERAGE(D153:D157)</f>
+        <v>13462.8</v>
+      </c>
+      <c r="H157" s="1">
+        <f>_xlfn.STDEV.S(D153:D157)</f>
+        <v>764.6359918287917</v>
+      </c>
+      <c r="I157" s="1">
+        <f>((SUM(D153:D157) - E157 - F157) / (COUNT(D153:D157) - 2))</f>
+        <v>13413.333333333334</v>
+      </c>
+    </row>
+    <row r="158" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A158" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="B158" t="s">
+        <v>66</v>
+      </c>
+      <c r="C158">
+        <v>1</v>
+      </c>
+      <c r="D158">
+        <v>13094</v>
+      </c>
+    </row>
+    <row r="159" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A159" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="B159" t="s">
+        <v>71</v>
+      </c>
+      <c r="C159">
+        <v>2</v>
+      </c>
+      <c r="D159">
+        <v>13214</v>
+      </c>
+    </row>
+    <row r="160" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A160" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="C160">
+        <v>3</v>
+      </c>
+      <c r="D160">
+        <v>11733</v>
+      </c>
+    </row>
+    <row r="161" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A161" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="C161">
+        <v>4</v>
+      </c>
+      <c r="D161">
+        <v>11951</v>
+      </c>
+    </row>
+    <row r="162" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A162" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="C162">
+        <v>5</v>
+      </c>
+      <c r="D162">
+        <v>11979</v>
+      </c>
+      <c r="E162" s="1">
+        <f>MAX(D158:D162)</f>
+        <v>13214</v>
+      </c>
+      <c r="F162" s="1">
+        <f>MIN(D158:D162)</f>
+        <v>11733</v>
+      </c>
+      <c r="G162" s="1">
+        <f>AVERAGE(D158:D162)</f>
+        <v>12394.2</v>
+      </c>
+      <c r="H162" s="1">
+        <f>_xlfn.STDEV.S(D158:D162)</f>
+        <v>701.39054741278051</v>
+      </c>
+      <c r="I162" s="1">
+        <f>((SUM(D158:D162) - E162 - F162) / (COUNT(D158:D162) - 2))</f>
+        <v>12341.333333333334</v>
+      </c>
+    </row>
+    <row r="163" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A163" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="B163" t="s">
+        <v>66</v>
+      </c>
+      <c r="C163">
+        <v>1</v>
+      </c>
+      <c r="D163">
+        <v>11334</v>
+      </c>
+    </row>
+    <row r="164" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A164" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="B164" t="s">
+        <v>71</v>
+      </c>
+      <c r="C164">
+        <v>2</v>
+      </c>
+      <c r="D164">
+        <v>15318</v>
+      </c>
+    </row>
+    <row r="165" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A165" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="B165" t="s">
+        <v>74</v>
+      </c>
+      <c r="C165">
+        <v>3</v>
+      </c>
+      <c r="D165">
+        <v>14860</v>
+      </c>
+    </row>
+    <row r="166" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A166" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="C166">
+        <v>4</v>
+      </c>
+      <c r="D166">
+        <v>14216</v>
+      </c>
+    </row>
+    <row r="167" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A167" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="C167">
+        <v>5</v>
+      </c>
+      <c r="D167">
+        <v>15438</v>
+      </c>
+      <c r="E167" s="1">
+        <f>MAX(D163:D167)</f>
+        <v>15438</v>
+      </c>
+      <c r="F167" s="1">
+        <f>MIN(D163:D167)</f>
+        <v>11334</v>
+      </c>
+      <c r="G167" s="1">
+        <f>AVERAGE(D163:D167)</f>
+        <v>14233.2</v>
+      </c>
+      <c r="H167" s="1">
+        <f>_xlfn.STDEV.S(D163:D167)</f>
+        <v>1690.1825936862526</v>
+      </c>
+      <c r="I167" s="1">
+        <f>((SUM(D163:D167) - E167 - F167) / (COUNT(D163:D167) - 2))</f>
+        <v>14798</v>
+      </c>
+    </row>
+    <row r="168" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A168" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="B168" t="s">
+        <v>73</v>
+      </c>
+      <c r="C168">
+        <v>6</v>
+      </c>
+      <c r="D168">
+        <v>11170</v>
+      </c>
+    </row>
+    <row r="169" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A169" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="C169">
+        <v>7</v>
+      </c>
+      <c r="D169">
+        <v>13838</v>
+      </c>
+    </row>
+    <row r="170" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A170" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="C170">
+        <v>8</v>
+      </c>
+      <c r="D170">
+        <v>11443</v>
+      </c>
+    </row>
+    <row r="171" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A171" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="C171">
+        <v>9</v>
+      </c>
+      <c r="D171">
+        <v>11705</v>
+      </c>
+    </row>
+    <row r="172" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A172" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="C172">
+        <v>10</v>
+      </c>
+      <c r="D172">
+        <v>11720</v>
+      </c>
+      <c r="E172" s="1">
+        <f>MAX(D168:D172)</f>
+        <v>13838</v>
+      </c>
+      <c r="F172" s="1">
+        <f>MIN(D168:D172)</f>
+        <v>11170</v>
+      </c>
+      <c r="G172" s="1">
+        <f>AVERAGE(D168:D172)</f>
+        <v>11975.2</v>
+      </c>
+      <c r="H172" s="1">
+        <f>_xlfn.STDEV.S(D168:D172)</f>
+        <v>1065.3336097204481</v>
+      </c>
+      <c r="I172" s="1">
+        <f>((SUM(D168:D172) - E172 - F172) / (COUNT(D168:D172) - 2))</f>
+        <v>11622.666666666666</v>
+      </c>
+    </row>
+    <row r="173" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A173" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="B173" t="s">
+        <v>75</v>
+      </c>
+      <c r="C173">
+        <v>11</v>
+      </c>
+      <c r="D173">
+        <v>10033</v>
+      </c>
+    </row>
+    <row r="174" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A174" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="C174">
+        <v>12</v>
+      </c>
+      <c r="D174">
+        <v>12205</v>
+      </c>
+    </row>
+    <row r="175" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A175" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="C175">
+        <v>13</v>
+      </c>
+      <c r="D175">
+        <v>12117</v>
+      </c>
+    </row>
+    <row r="176" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A176" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="C176">
+        <v>14</v>
+      </c>
+      <c r="D176">
+        <v>12128</v>
+      </c>
+    </row>
+    <row r="177" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A177" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="C177">
+        <v>15</v>
+      </c>
+      <c r="D177">
+        <v>12488</v>
+      </c>
+      <c r="E177" s="1">
+        <f>MAX(D173:D177)</f>
+        <v>12488</v>
+      </c>
+      <c r="F177" s="1">
+        <f>MIN(D173:D177)</f>
+        <v>10033</v>
+      </c>
+      <c r="G177" s="1">
+        <f>AVERAGE(D173:D177)</f>
+        <v>11794.2</v>
+      </c>
+      <c r="H177" s="1">
+        <f>_xlfn.STDEV.S(D173:D177)</f>
+        <v>995.93709640719783</v>
+      </c>
+      <c r="I177" s="1">
+        <f>((SUM(D173:D177) - E177 - F177) / (COUNT(D173:D177) - 2))</f>
+        <v>12150</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>